<commit_message>
Navigation for account tab created
</commit_message>
<xml_diff>
--- a/Error-Exceptionlog.xlsx
+++ b/Error-Exceptionlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>S.No</t>
   </si>
@@ -150,13 +150,22 @@
   </si>
   <si>
     <t>Unsatisfied dependency expressed through field 'accessible'</t>
+  </si>
+  <si>
+    <t>Opened H2 console before launching app</t>
+  </si>
+  <si>
+    <t>org.h2.jdbc.JdbcSQLException: Connection is broken: "java.net.ConnectException: Connection refused: connect: localhost</t>
+  </si>
+  <si>
+    <t>Restarted H2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +209,12 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,7 +268,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -290,6 +305,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -564,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -810,13 +826,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="2" max="2" width="106.28515625" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" customWidth="1"/>
     <col min="5" max="10" width="9.140625" customWidth="1"/>
@@ -854,6 +870,20 @@
       </c>
       <c r="B3" s="15" t="s">
         <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
Completed CRUD for supplier and product
</commit_message>
<xml_diff>
--- a/Error-Exceptionlog.xlsx
+++ b/Error-Exceptionlog.xlsx
@@ -580,7 +580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -826,7 +826,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -887,6 +887,9 @@
       </c>
     </row>
     <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="D5" s="16"/>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1"/>

</xml_diff>